<commit_message>
Initial changes during R3
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -647,7 +647,7 @@
     <t xml:space="preserve">l$threepsm_cf_p</t>
   </si>
   <si>
-    <t xml:space="preserve">.812</t>
+    <t xml:space="preserve">.807</t>
   </si>
   <si>
     <t xml:space="preserve">l$egger_df_p</t>
@@ -659,7 +659,7 @@
     <t xml:space="preserve">l$threepsm_df_p</t>
   </si>
   <si>
-    <t xml:space="preserve">.706</t>
+    <t xml:space="preserve">.701</t>
   </si>
   <si>
     <t xml:space="preserve">l$egger_bf_p</t>
@@ -671,7 +671,7 @@
     <t xml:space="preserve">l$threepsm_bf_p</t>
   </si>
   <si>
-    <t xml:space="preserve">.271</t>
+    <t xml:space="preserve">.274</t>
   </si>
   <si>
     <t xml:space="preserve">behav_df_below_4</t>

</xml_diff>